<commit_message>
optimisation des ressources DataMover vs Interconnect
git-svn-id: http://einstein/svn/firmware/FIR-00251-Output/trunk@26374 3e98269d-ff51-e449-abca-491a6567d830
</commit_message>
<xml_diff>
--- a/src/FB DDR interfaces throughput.xlsx
+++ b/src/FB DDR interfaces throughput.xlsx
@@ -221,7 +221,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -521,7 +532,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,11 +627,11 @@
         <v>800</v>
       </c>
       <c r="B10" s="6">
-        <v>0.85</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="C10" s="1">
         <f>A10*B10</f>
-        <v>680</v>
+        <v>668</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,7 +702,7 @@
       </c>
       <c r="C21" s="7">
         <f>IF($B25 &lt; $C$10,B21,($C$10-$C22-$C24)/2)</f>
-        <v>287.71960000000001</v>
+        <v>281.71960000000001</v>
       </c>
       <c r="D21" s="8">
         <f>B18/(B21*1000000)</f>
@@ -699,7 +710,7 @@
       </c>
       <c r="E21" s="9">
         <f>(B21-C21)*1000000*D21 / 4</f>
-        <v>12645.706164705878</v>
+        <v>14097.000282352938</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -727,15 +738,15 @@
       </c>
       <c r="C23" s="7">
         <f>IF($B25 &lt; $C$10,B23,($C$10-$C22-$C24)/2)</f>
-        <v>287.71960000000001</v>
+        <v>281.71960000000001</v>
       </c>
       <c r="D23" s="8">
         <f>B19/(B23*1000000)</f>
         <v>9.6752941176470584E-4</v>
       </c>
       <c r="E23" s="9">
-        <f t="shared" ref="E22:E23" si="0">(B23-C23)*1000000*D23 / 4</f>
-        <v>12645.706164705878</v>
+        <f t="shared" ref="E23" si="0">(B23-C23)*1000000*D23 / 4</f>
+        <v>14097.000282352938</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -763,7 +774,7 @@
       </c>
       <c r="C25" s="11">
         <f>SUM(C21:C24)</f>
-        <v>680</v>
+        <v>668</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,7 +825,7 @@
       </c>
       <c r="C32" s="7">
         <f>IF($B36 &lt; $C$10,B32,($C$10-$C33-$C35)/2)</f>
-        <v>277.88920000000002</v>
+        <v>271.88920000000002</v>
       </c>
       <c r="D32" s="8">
         <f>B29/(B32*1000000)</f>
@@ -822,7 +833,7 @@
       </c>
       <c r="E32" s="9">
         <f>(B32-C32)*1000000*D32 / 4</f>
-        <v>43205.680799999987</v>
+        <v>49361.680799999987</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -850,7 +861,7 @@
       </c>
       <c r="C34" s="7">
         <f>IF($B36 &lt; $C$10,B34,($C$10-$C33-$C35)/2)</f>
-        <v>277.88920000000002</v>
+        <v>271.88920000000002</v>
       </c>
       <c r="D34" s="8">
         <f>B30/(B34*1000000)</f>
@@ -858,7 +869,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" ref="E34" si="1">(B34-C34)*1000000*D34 / 4</f>
-        <v>43205.680799999987</v>
+        <v>49361.680799999987</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -886,7 +897,7 @@
       </c>
       <c r="C36" s="11">
         <f>SUM(C32:C35)</f>
-        <v>680</v>
+        <v>668</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -937,7 +948,7 @@
       </c>
       <c r="C43" s="7">
         <f>IF($B47 &lt; $C$10,B43,($C$10-$C44-$C46)/2)</f>
-        <v>253.31319999999999</v>
+        <v>247.31319999999999</v>
       </c>
       <c r="D43" s="8">
         <f>B40/(B43*1000000)</f>
@@ -945,7 +956,7 @@
       </c>
       <c r="E43" s="9">
         <f>(B43-C43)*1000000*D43 / 4</f>
-        <v>70361.654400000014</v>
+        <v>86181.082971428579</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,7 +984,7 @@
       </c>
       <c r="C45" s="7">
         <f>IF($B47 &lt; $C$10,B45,($C$10-$C44-$C46)/2)</f>
-        <v>253.31319999999999</v>
+        <v>247.31319999999999</v>
       </c>
       <c r="D45" s="8">
         <f>B41/(B45*1000000)</f>
@@ -981,7 +992,7 @@
       </c>
       <c r="E45" s="9">
         <f t="shared" ref="E45" si="2">(B45-C45)*1000000*D45 / 4</f>
-        <v>70361.654400000014</v>
+        <v>86181.082971428579</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1009,10 +1020,15 @@
       </c>
       <c r="C47" s="11">
         <f>SUM(C43:C46)</f>
-        <v>680</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E21 E23 E32 E34 E43 E45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>16384</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>